<commit_message>
Created Wanted List Python Program
</commit_message>
<xml_diff>
--- a/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Agustus 2021 - 3 Oktober 2021).xlsx
+++ b/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Agustus 2021 - 3 Oktober 2021).xlsx
@@ -4554,7 +4554,11 @@
       </c>
       <c r="Y35" s="45" t="inlineStr"/>
       <c r="Z35" s="57" t="inlineStr"/>
-      <c r="AA35" s="45" t="inlineStr"/>
+      <c r="AA35" s="49" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="15.6" customHeight="1">
       <c r="A36" s="33" t="n">

</xml_diff>